<commit_message>
Did it in d3
</commit_message>
<xml_diff>
--- a/Excel/cars-sample_Excel_scatterplot.xlsx
+++ b/Excel/cars-sample_Excel_scatterplot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GenericFiles\Documents\573\02-datavis-7ways-1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD3D611-96DD-4D61-B744-91D533806C1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF484F2E-5F46-4CC1-BBEB-4AA104593270}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScatterPlot" sheetId="1" r:id="rId1"/>
@@ -7325,11 +7325,11 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.91902</cdr:x>
+      <cdr:x>0.91329</cdr:x>
       <cdr:y>0.61202</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.9865</cdr:x>
+      <cdr:x>0.98077</cdr:x>
       <cdr:y>0.74464</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -7345,8 +7345,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8431531" y="4131945"/>
-          <a:ext cx="619125" cy="895350"/>
+          <a:off x="8318281" y="4293939"/>
+          <a:ext cx="614610" cy="930463"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7401,12 +7401,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.93559</cdr:x>
-      <cdr:y>0.61693</cdr:y>
+      <cdr:x>0.92528</cdr:x>
+      <cdr:y>0.62139</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>1</cdr:x>
-      <cdr:y>0.7481</cdr:y>
+      <cdr:x>0.98969</cdr:x>
+      <cdr:y>0.75256</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -7421,8 +7421,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8578216" y="4170936"/>
-          <a:ext cx="590549" cy="886824"/>
+          <a:off x="8427446" y="4359704"/>
+          <a:ext cx="586649" cy="920290"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7457,11 +7457,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.92293</cdr:x>
+      <cdr:x>0.90803</cdr:x>
       <cdr:y>0.62821</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.93955</cdr:x>
+      <cdr:x>0.92465</cdr:x>
       <cdr:y>0.64795</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -7477,12 +7477,15 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8462168" y="4247222"/>
-          <a:ext cx="152368" cy="133500"/>
+          <a:off x="8270384" y="4407528"/>
+          <a:ext cx="151376" cy="138496"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
@@ -7503,6 +7506,195 @@
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.90984</cdr:x>
+      <cdr:y>0.59017</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98548</cdr:x>
+      <cdr:y>0.62142</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A76A233-6C07-4D8C-8E5E-C99AD2FF2569}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8286856" y="4140661"/>
+          <a:ext cx="688931" cy="219206"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Weight</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.9018</cdr:x>
+      <cdr:y>0.66605</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93161</cdr:x>
+      <cdr:y>0.70393</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="Oval 6">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30523077-7999-447A-B6CF-3C387E06B43F}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8213594" y="4673017"/>
+          <a:ext cx="271589" cy="265731"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:endParaRPr lang="en-US"/>
         </a:p>

</xml_diff>